<commit_message>
All infomration in researcher area
</commit_message>
<xml_diff>
--- a/upload/data.xlsx
+++ b/upload/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63" count="63">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107" count="107">
   <x:si>
     <x:t>logFileID</x:t>
   </x:si>
@@ -203,6 +203,138 @@
   </x:si>
   <x:si>
     <x:t>March 28th 2017, 1:08:22 pm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sml5527</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q: issFav Q: issOpp Q: candFav Q: candFav Q: undefined Q: undefined</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490795173254</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35_1_18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q: issFav Q: issOpp Q: candFav Q: candOpp Q: undefined Q: undefined</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490795188179</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q: issFav Q: issOpp Q: candFav Q: undefined Q: candOpp Q: undefined</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490795244453</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Work Out</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490795434798</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Community Service</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490795440705</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490796534323</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490796537647</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490796539788</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490796541557</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Compete in Game Tournament</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798333236</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798335895</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798338336</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798340766</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798345830</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798353222</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798384022</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798388102</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798394634</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798399735</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Meet the Robotics Team</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798410462</x:t>
+  </x:si>
+  <x:si>
+    <x:t>endGame</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Winner: Martian Dog Player Rank:6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490798743808</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Q: issFav Q: issOpp Q: candFav Q: candOpp Q: candOpp Q: undefined</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490799704713</x:t>
+  </x:si>
+  <x:si>
+    <x:t>35_1_19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490801937885</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490802115079</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490802123585</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490802140752</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Study in the Library</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490802146655</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1490802151791</x:t>
+  </x:si>
+  <x:si>
+    <x:t>March 30th 2017, 12:41:14 pm</x:t>
+  </x:si>
+  <x:si>
+    <x:t>March 30th 2017, 12:41:53 pm</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1255,6 +1387,696 @@
         <x:v>61</x:v>
       </x:c>
     </x:row>
+    <x:row r="31" spans="1:7">
+      <x:c r="A31" s="0" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="F31" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="G31" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:7">
+      <x:c r="A32" s="0" t="n">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="F32" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="G32" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:7">
+      <x:c r="A33" s="0" t="n">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="F33" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="G33" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:7">
+      <x:c r="A34" s="0" t="n">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="F34" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="G34" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:7">
+      <x:c r="A35" s="0" t="n">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="F35" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="G35" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:7">
+      <x:c r="A36" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="F36" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="G36" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:7">
+      <x:c r="A37" s="0" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F37" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="G37" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:7">
+      <x:c r="A38" s="0" t="n">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F38" s="0" t="s">
+        <x:v>77</x:v>
+      </x:c>
+      <x:c r="G38" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:7">
+      <x:c r="A39" s="0" t="n">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F39" s="0" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="G39" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:7">
+      <x:c r="A40" s="0" t="n">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F40" s="0" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="G40" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:7">
+      <x:c r="A41" s="0" t="n">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F41" s="0" t="s">
+        <x:v>81</x:v>
+      </x:c>
+      <x:c r="G41" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:7">
+      <x:c r="A42" s="0" t="n">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F42" s="0" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="G42" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:7">
+      <x:c r="A43" s="0" t="n">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F43" s="0" t="s">
+        <x:v>83</x:v>
+      </x:c>
+      <x:c r="G43" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:7">
+      <x:c r="A44" s="0" t="n">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F44" s="0" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="G44" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:7">
+      <x:c r="A45" s="0" t="n">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F45" s="0" t="s">
+        <x:v>85</x:v>
+      </x:c>
+      <x:c r="G45" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:7">
+      <x:c r="A46" s="0" t="n">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F46" s="0" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="G46" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:7">
+      <x:c r="A47" s="0" t="n">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="F47" s="0" t="s">
+        <x:v>87</x:v>
+      </x:c>
+      <x:c r="G47" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:7">
+      <x:c r="A48" s="0" t="n">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F48" s="0" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="G48" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:7">
+      <x:c r="A49" s="0" t="n">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F49" s="0" t="s">
+        <x:v>89</x:v>
+      </x:c>
+      <x:c r="G49" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:7">
+      <x:c r="A50" s="0" t="n">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="F50" s="0" t="s">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="G50" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:7">
+      <x:c r="A51" s="0" t="n">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="F51" s="0" t="s">
+        <x:v>94</x:v>
+      </x:c>
+      <x:c r="G51" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:7">
+      <x:c r="A52" s="0" t="n">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E52" s="0" t="s">
+        <x:v>95</x:v>
+      </x:c>
+      <x:c r="F52" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="G52" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:7">
+      <x:c r="A53" s="0" t="n">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E53" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="F53" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="G53" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:7">
+      <x:c r="A54" s="0" t="n">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E54" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="F54" s="0" t="s">
+        <x:v>99</x:v>
+      </x:c>
+      <x:c r="G54" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:7">
+      <x:c r="A55" s="0" t="n">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E55" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="F55" s="0" t="s">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="G55" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:7">
+      <x:c r="A56" s="0" t="n">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D56" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E56" s="0" t="s">
+        <x:v>79</x:v>
+      </x:c>
+      <x:c r="F56" s="0" t="s">
+        <x:v>101</x:v>
+      </x:c>
+      <x:c r="G56" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:7">
+      <x:c r="A57" s="0" t="n">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D57" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E57" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="F57" s="0" t="s">
+        <x:v>103</x:v>
+      </x:c>
+      <x:c r="G57" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:7">
+      <x:c r="A58" s="0" t="n">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="n">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="D58" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E58" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="F58" s="0" t="s">
+        <x:v>104</x:v>
+      </x:c>
+      <x:c r="G58" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:7">
+      <x:c r="A59" s="0" t="n">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E59" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="F59" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="G59" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="60" spans="1:7">
+      <x:c r="A60" s="0" t="n">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E60" s="0" t="s">
+        <x:v>102</x:v>
+      </x:c>
+      <x:c r="F60" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="G60" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>